<commit_message>
feat: import siswa from excel(un finished)
fix #51
</commit_message>
<xml_diff>
--- a/format_import_siswa.xlsx
+++ b/format_import_siswa.xlsx
@@ -38,10 +38,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>TrianNurizkillah</t>
-  </si>
-  <si>
-    <t>triannurizkillah@gmail.com</t>
+    <t>TrianNurizkillah4</t>
+  </si>
+  <si>
+    <t>triannurizkillah4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -373,7 +373,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix: import/post/put data getting error when update state in datatable
from backend add status 201 with data join table

fix #46
fix #51
</commit_message>
<xml_diff>
--- a/format_import_siswa.xlsx
+++ b/format_import_siswa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>No</t>
   </si>
@@ -42,6 +42,15 @@
   </si>
   <si>
     <t>triannurizkillah4@gmail.com</t>
+  </si>
+  <si>
+    <t>rdfd</t>
+  </si>
+  <si>
+    <t>TrianNurizkillah6</t>
+  </si>
+  <si>
+    <t>triannurizkillah6@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -370,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,9 +420,24 @@
         <v>12345678</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>